<commit_message>
Refine Resume Filter: multi-keyword search, UI improvements, and 104 unique sample resumes
</commit_message>
<xml_diff>
--- a/my_app/uploads/data.xlsx
+++ b/my_app/uploads/data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF104"/>
+  <dimension ref="A1:AG107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:AF104"/>
@@ -582,6 +582,11 @@
           <t>Reject Mail Sent</t>
         </is>
       </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>Screened By</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -611,7 +616,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://example.com/resume/johndoe</t>
+          <t>Resume_JohnDoe_2.pdf</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -724,6 +729,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -753,7 +759,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://example.com/resume/janesmith</t>
+          <t>Resume_JaneSmith_3.pdf</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -848,7 +854,11 @@
       </c>
       <c r="Y3" t="inlineStr"/>
       <c r="Z3" t="inlineStr"/>
-      <c r="AA3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>{"Communication":"good","Technical Assessment":"good","Problem-Solving":"good","Overall Potential":"good","Recommendation":"Proceed Round 2"}</t>
+        </is>
+      </c>
       <c r="AB3" t="inlineStr"/>
       <c r="AC3" t="inlineStr"/>
       <c r="AD3" t="inlineStr">
@@ -862,6 +872,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>ashwin</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -889,7 +904,11 @@
           <t>https://linkedin.com/in/samwilson</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Resume_Ram_4.pdf</t>
+        </is>
+      </c>
       <c r="G4" t="inlineStr">
         <is>
           <t>UI/UX Designer</t>
@@ -996,6 +1015,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1025,7 +1045,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://example.com/resume/xbal</t>
+          <t>Resume_ArhaanKapadia_5.pdf</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -1086,6 +1106,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1115,7 +1136,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://example.com/resume/nsachdev</t>
+          <t>Resume_LakshitBasak_6.pdf</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -1176,6 +1197,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1205,7 +1227,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://example.com/resume/choudharyahana</t>
+          <t>Resume_BijuArora_7.pdf</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -1266,6 +1288,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1295,7 +1318,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://example.com/resume/wbahri</t>
+          <t>Resume_ArmaanJayaraman_8.pdf</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -1356,6 +1379,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1385,7 +1409,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://example.com/resume/kairashankar</t>
+          <t>Resume_MohanlalHans_9.pdf</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -1446,11 +1470,12 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-02-18 00:47:00</t>
+          <t>2/18/2025</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1475,7 +1500,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://example.com/resume/bariayuvaan</t>
+          <t>Resume_RohanVohra_10.pdf</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -1516,17 +1541,33 @@
       <c r="R10" t="inlineStr"/>
       <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr"/>
-      <c r="U10" t="inlineStr"/>
-      <c r="V10" t="inlineStr"/>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>Applied</t>
+        </is>
+      </c>
       <c r="W10" t="inlineStr">
         <is>
-          <t>New</t>
+          <t>Proceed Further</t>
         </is>
       </c>
       <c r="X10" t="inlineStr"/>
-      <c r="Y10" t="inlineStr"/>
+      <c r="Y10" t="inlineStr">
+        <is>
+          <t>good candidate</t>
+        </is>
+      </c>
       <c r="Z10" t="inlineStr"/>
-      <c r="AA10" t="inlineStr"/>
+      <c r="AA10" t="inlineStr">
+        <is>
+          <t>{"Communication":"good ","Technical Assessment":"good","Problem-Solving":"good","Overall Potential":"good","Recommendation":""}</t>
+        </is>
+      </c>
       <c r="AB10" t="inlineStr"/>
       <c r="AC10" t="inlineStr"/>
       <c r="AD10" t="inlineStr"/>
@@ -1536,6 +1577,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG10" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1565,7 +1611,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>https://example.com/resume/hiran68</t>
+          <t>Resume_NayantaraKapadia_11.pdf</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1626,6 +1672,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1655,7 +1702,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>https://example.com/resume/ela56</t>
+          <t>Resume_FarhanBassi_12.pdf</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1716,6 +1763,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1745,7 +1793,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>https://example.com/resume/viswanathanalia</t>
+          <t>Resume_AnayBail_13.pdf</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1806,6 +1854,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1835,7 +1884,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>https://example.com/resume/tvora</t>
+          <t>Resume_MadhavBoase_14.pdf</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1896,6 +1945,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1925,7 +1975,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>https://example.com/resume/devansh64</t>
+          <t>Resume_NakulSrinivas_15.pdf</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1986,6 +2036,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2015,7 +2066,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>https://example.com/resume/vaidyasahil</t>
+          <t>Resume_AzadKar_16.pdf</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -2076,6 +2127,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2105,7 +2157,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>https://example.com/resume/auroraira</t>
+          <t>Resume_IvanaSingh_17.pdf</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -2166,6 +2218,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2195,7 +2248,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>https://example.com/resume/tramakrishnan</t>
+          <t>Resume_HeerBuch_18.pdf</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -2256,6 +2309,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2285,7 +2339,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>https://example.com/resume/ramaswamymiraya</t>
+          <t>Resume_TaraAgate_19.pdf</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -2346,6 +2400,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2375,7 +2430,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>https://example.com/resume/trisha70</t>
+          <t>Resume_SaanviChawla_20.pdf</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -2436,6 +2491,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2465,7 +2521,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>https://example.com/resume/kiaan96</t>
+          <t>Resume_AliaKadakia_21.pdf</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -2526,6 +2582,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2555,7 +2612,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>https://example.com/resume/zoyamann</t>
+          <t>Resume_BhavinSethi_22.pdf</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -2616,6 +2673,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2645,7 +2703,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>https://example.com/resume/rohanranganathan</t>
+          <t>Resume_NakulGhose_23.pdf</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -2706,6 +2764,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2735,7 +2794,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>https://example.com/resume/taimurarya</t>
+          <t>Resume_AdiraBhatia_24.pdf</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -2796,6 +2855,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2825,7 +2885,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>https://example.com/resume/wreddy</t>
+          <t>Resume_DevanshRastogi_25.pdf</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -2886,6 +2946,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2915,7 +2976,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>https://example.com/resume/riaandeo</t>
+          <t>Resume_IvanaSuresh_26.pdf</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -2976,6 +3037,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3005,7 +3067,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>https://example.com/resume/sherealia</t>
+          <t>Resume_MyraSha_27.pdf</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -3066,6 +3128,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3095,7 +3158,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>https://example.com/resume/madhup70</t>
+          <t>Resume_KabirVerma_28.pdf</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -3156,6 +3219,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3185,7 +3249,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>https://example.com/resume/lakshaymane</t>
+          <t>Resume_VedikaChahal_29.pdf</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -3246,6 +3310,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3275,7 +3340,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>https://example.com/resume/krishnatiya</t>
+          <t>Resume_AarnaShah_30.pdf</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -3336,6 +3401,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3365,7 +3431,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>https://example.com/resume/sahiltata</t>
+          <t>Resume_SahilRatti_31.pdf</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -3426,6 +3492,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3455,7 +3522,7 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>https://example.com/resume/shamik49</t>
+          <t>Resume_DharmajanDatta_32.pdf</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -3516,6 +3583,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3545,7 +3613,7 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>https://example.com/resume/yasminbabu</t>
+          <t>Resume_MadhavRaval_33.pdf</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -3606,6 +3674,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3635,7 +3704,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>https://example.com/resume/yashvikala</t>
+          <t>Resume_TaimurBhatnagar_34.pdf</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
@@ -3696,6 +3765,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3725,7 +3795,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>https://example.com/resume/jchanda</t>
+          <t>Resume_IndransGuha_35.pdf</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -3786,6 +3856,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3815,7 +3886,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>https://example.com/resume/vaibhavsule</t>
+          <t>Resume_DaminiMann_36.pdf</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
@@ -3876,6 +3947,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -3905,7 +3977,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>https://example.com/resume/cherianjayan</t>
+          <t>Resume_BadalManda_37.pdf</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
@@ -3966,6 +4038,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -3995,7 +4068,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>https://example.com/resume/eviswanathan</t>
+          <t>Resume_SuhanaKala_38.pdf</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
@@ -4056,6 +4129,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -4085,7 +4159,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>https://example.com/resume/lmagar</t>
+          <t>Resume_NakulShetty_39.pdf</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -4146,6 +4220,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -4175,7 +4250,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>https://example.com/resume/kiberhea</t>
+          <t>Resume_IshaanLanka_40.pdf</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -4236,6 +4311,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -4265,7 +4341,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>https://example.com/resume/wsarraf</t>
+          <t>Resume_PranayBarad_41.pdf</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
@@ -4326,6 +4402,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -4355,7 +4432,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>https://example.com/resume/vchander</t>
+          <t>Resume_ElakshiSha_42.pdf</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
@@ -4416,6 +4493,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -4445,7 +4523,7 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>https://example.com/resume/srajagopalan</t>
+          <t>Resume_BaijuTak_43.pdf</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
@@ -4506,6 +4584,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -4535,7 +4614,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>https://example.com/resume/routzoya</t>
+          <t>Resume_PrerakKapoor_44.pdf</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
@@ -4596,6 +4675,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -4625,7 +4705,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>https://example.com/resume/kalakavya</t>
+          <t>Resume_AdiraChauhan_45.pdf</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
@@ -4686,6 +4766,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -4715,7 +4796,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>https://example.com/resume/renee59</t>
+          <t>Resume_BhavinChaudhary_46.pdf</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
@@ -4776,6 +4857,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -4805,7 +4887,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>https://example.com/resume/warriormadhup</t>
+          <t>Resume_ManjariKibe_47.pdf</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
@@ -4866,6 +4948,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -4895,7 +4978,7 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>https://example.com/resume/jayant22</t>
+          <t>Resume_AbramBahl_48.pdf</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
@@ -4956,6 +5039,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -4985,7 +5069,7 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>https://example.com/resume/kiara34</t>
+          <t>Resume_MishtiBala_49.pdf</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
@@ -5046,6 +5130,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -5075,7 +5160,7 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>https://example.com/resume/daninishith</t>
+          <t>Resume_DaminiBhakta_50.pdf</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
@@ -5136,6 +5221,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -5165,7 +5251,7 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>https://example.com/resume/kannannehmat</t>
+          <t>Resume_GatikSrivastava_51.pdf</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
@@ -5226,6 +5312,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -5255,7 +5342,7 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>https://example.com/resume/rdeshmukh</t>
+          <t>Resume_AnikaBala_52.pdf</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
@@ -5316,6 +5403,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -5345,7 +5433,7 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>https://example.com/resume/siya00</t>
+          <t>Resume_HiranBansal_53.pdf</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
@@ -5406,6 +5494,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -5435,7 +5524,7 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>https://example.com/resume/deoelakshi</t>
+          <t>Resume_PihuVora_54.pdf</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
@@ -5496,6 +5585,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -5525,7 +5615,7 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>https://example.com/resume/semadvika</t>
+          <t>Resume_KhushiSuri_55.pdf</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
@@ -5586,6 +5676,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -5615,7 +5706,7 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>https://example.com/resume/darshitvarughese</t>
+          <t>Resume_AniruddhKhosla_56.pdf</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
@@ -5676,6 +5767,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -5705,7 +5797,7 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>https://example.com/resume/ramaswamydamini</t>
+          <t>Resume_LavanyaVaidya_57.pdf</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
@@ -5766,6 +5858,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -5795,7 +5888,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>https://example.com/resume/arandhawa</t>
+          <t>Resume_NayantaraUppal_58.pdf</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
@@ -5856,6 +5949,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -5885,7 +5979,7 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>https://example.com/resume/onkar05</t>
+          <t>Resume_VeerKalita_59.pdf</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
@@ -5946,6 +6040,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -5975,7 +6070,7 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>https://example.com/resume/lallariaan</t>
+          <t>Resume_IndransSawhney_60.pdf</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
@@ -6036,6 +6131,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -6065,7 +6161,7 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>https://example.com/resume/xaurora</t>
+          <t>Resume_MannatBalan_61.pdf</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
@@ -6126,6 +6222,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -6155,7 +6252,7 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>https://example.com/resume/jivin10</t>
+          <t>Resume_DharmajanZachariah_62.pdf</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
@@ -6216,6 +6313,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -6245,7 +6343,7 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>https://example.com/resume/dhanukgrover</t>
+          <t>Resume_GokulShah_63.pdf</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
@@ -6306,6 +6404,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -6335,7 +6434,7 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>https://example.com/resume/rhea39</t>
+          <t>Resume_MahikaDora_64.pdf</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
@@ -6396,6 +6495,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -6425,7 +6525,7 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>https://example.com/resume/manimohanlal</t>
+          <t>Resume_BijuLuthra_65.pdf</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
@@ -6486,6 +6586,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -6515,7 +6616,7 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>https://example.com/resume/nirvisant</t>
+          <t>Resume_IndransSetty_66.pdf</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
@@ -6576,6 +6677,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -6605,7 +6707,7 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>https://example.com/resume/akarshjha</t>
+          <t>Resume_TariniVaidya_67.pdf</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
@@ -6666,6 +6768,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -6695,7 +6798,7 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>https://example.com/resume/subramaniantrisha</t>
+          <t>Resume_DhanushBahri_68.pdf</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
@@ -6756,6 +6859,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -6785,7 +6889,7 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>https://example.com/resume/seshadriira</t>
+          <t>Resume_SumerSubramanian_69.pdf</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
@@ -6846,6 +6950,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -6875,7 +6980,7 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>https://example.com/resume/bandianika</t>
+          <t>Resume_KimayaBhatia_70.pdf</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
@@ -6936,6 +7041,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -6965,7 +7071,7 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>https://example.com/resume/aswamy</t>
+          <t>Resume_AarushJayaraman_71.pdf</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
@@ -7026,6 +7132,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -7055,7 +7162,7 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>https://example.com/resume/hirankrish</t>
+          <t>Resume_HazelBen_72.pdf</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
@@ -7116,6 +7223,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -7145,7 +7253,7 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>https://example.com/resume/farhan33</t>
+          <t>Resume_HiranKuruvilla_73.pdf</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
@@ -7206,6 +7314,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -7235,7 +7344,7 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>https://example.com/resume/lsalvi</t>
+          <t>Resume_YuvaanSinghal_74.pdf</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
@@ -7296,6 +7405,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -7325,7 +7435,7 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>https://example.com/resume/jayeshrajagopalan</t>
+          <t>Resume_HeerMani_75.pdf</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
@@ -7386,6 +7496,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -7415,7 +7526,7 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>https://example.com/resume/anahishanker</t>
+          <t>Resume_NitaraBansal_76.pdf</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
@@ -7476,6 +7587,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -7505,7 +7617,7 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>https://example.com/resume/usabharwal</t>
+          <t>Resume_MyraDhar_77.pdf</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
@@ -7566,6 +7678,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -7595,7 +7708,7 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>https://example.com/resume/rajujivin</t>
+          <t>Resume_VaibhavDey_78.pdf</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
@@ -7656,6 +7769,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -7685,7 +7799,7 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>https://example.com/resume/samairachakrabarti</t>
+          <t>Resume_VihaanGade_79.pdf</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
@@ -7746,6 +7860,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -7775,7 +7890,7 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>https://example.com/resume/vghose</t>
+          <t>Resume_UrviLal_80.pdf</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
@@ -7836,6 +7951,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -7865,7 +7981,7 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>https://example.com/resume/psane</t>
+          <t>Resume_BijuBatta_81.pdf</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
@@ -7926,6 +8042,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -7955,7 +8072,7 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>https://example.com/resume/walladarshit</t>
+          <t>Resume_BhavinDatta_82.pdf</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
@@ -8016,6 +8133,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -8045,7 +8163,7 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>https://example.com/resume/ncomar</t>
+          <t>Resume_ManjariGolla_83.pdf</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
@@ -8106,6 +8224,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -8135,7 +8254,7 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>https://example.com/resume/bhaminisaini</t>
+          <t>Resume_ZainSura_84.pdf</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
@@ -8196,6 +8315,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -8225,7 +8345,7 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>https://example.com/resume/btripathi</t>
+          <t>Resume_DharmajanSen_85.pdf</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
@@ -8286,6 +8406,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -8315,7 +8436,7 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>https://example.com/resume/stuvanswamy</t>
+          <t>Resume_RohanKothari_86.pdf</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
@@ -8376,6 +8497,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -8405,7 +8527,7 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>https://example.com/resume/kiara85</t>
+          <t>Resume_AnviDutt_87.pdf</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
@@ -8466,6 +8588,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -8495,7 +8618,7 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>https://example.com/resume/nravel</t>
+          <t>Resume_AayushMani_88.pdf</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
@@ -8556,6 +8679,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -8585,7 +8709,7 @@
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>https://example.com/resume/qbal</t>
+          <t>Resume_GokulKhosla_89.pdf</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
@@ -8646,6 +8770,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -8675,7 +8800,7 @@
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>https://example.com/resume/faiyazkeer</t>
+          <t>Resume_SamihaKarpe_90.pdf</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
@@ -8736,6 +8861,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -8765,7 +8891,7 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>https://example.com/resume/kgrewal</t>
+          <t>Resume_ElaWarrior_91.pdf</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
@@ -8826,6 +8952,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -8855,7 +8982,7 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>https://example.com/resume/ayeshachana</t>
+          <t>Resume_ElaDevan_92.pdf</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
@@ -8916,6 +9043,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -8945,7 +9073,7 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>https://example.com/resume/dharmajanuppal</t>
+          <t>Resume_SamarthDhawan_93.pdf</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
@@ -9006,6 +9134,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -9035,7 +9164,7 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>https://example.com/resume/rasha30</t>
+          <t>Resume_ReyanshBorah_94.pdf</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
@@ -9096,6 +9225,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -9125,7 +9255,7 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>https://example.com/resume/anvibahri</t>
+          <t>Resume_ShlokGulati_95.pdf</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
@@ -9186,6 +9316,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -9215,7 +9346,7 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>https://example.com/resume/tara42</t>
+          <t>Resume_NeysaLalla_96.pdf</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
@@ -9276,6 +9407,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -9305,7 +9437,7 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>https://example.com/resume/hsamra</t>
+          <t>Resume_FaiyazJaggi_97.pdf</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
@@ -9366,6 +9498,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -9395,7 +9528,7 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>https://example.com/resume/trisha63</t>
+          <t>Resume_AdvikaBassi_98.pdf</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
@@ -9456,6 +9589,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -9485,7 +9619,7 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>https://example.com/resume/balmiraya</t>
+          <t>Resume_ZeeshanKrish_99.pdf</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
@@ -9546,6 +9680,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -9575,7 +9710,7 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>https://example.com/resume/lallanishith</t>
+          <t>Resume_JiyaDe_100.pdf</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
@@ -9636,6 +9771,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -9665,7 +9801,7 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>https://example.com/resume/ojas60</t>
+          <t>Resume_DivijChaudhuri_101.pdf</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
@@ -9726,6 +9862,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -9755,7 +9892,7 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>https://example.com/resume/buchstuvan</t>
+          <t>Resume_KismatBorah_102.pdf</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
@@ -9816,6 +9953,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -9845,7 +9983,7 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>https://example.com/resume/chaudharireyansh</t>
+          <t>Resume_MamootyKale_103.pdf</t>
         </is>
       </c>
       <c r="G103" t="inlineStr">
@@ -9906,6 +10044,7 @@
           <t>No</t>
         </is>
       </c>
+      <c r="AG103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -9935,7 +10074,7 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>https://example.com/resume/jhanvi85</t>
+          <t>Resume_GatikAndra_104.pdf</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
@@ -9996,6 +10135,136 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="AG104" t="inlineStr"/>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr"/>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>samp</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr"/>
+      <c r="D105" t="inlineStr"/>
+      <c r="E105" t="inlineStr"/>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>Resume_samp_105.pdf</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr"/>
+      <c r="H105" t="inlineStr"/>
+      <c r="I105" t="inlineStr"/>
+      <c r="J105" t="inlineStr"/>
+      <c r="K105" t="inlineStr"/>
+      <c r="L105" t="inlineStr"/>
+      <c r="M105" t="inlineStr"/>
+      <c r="N105" t="inlineStr"/>
+      <c r="O105" t="inlineStr"/>
+      <c r="P105" t="inlineStr"/>
+      <c r="Q105" t="inlineStr"/>
+      <c r="R105" t="inlineStr"/>
+      <c r="S105" t="inlineStr"/>
+      <c r="T105" t="inlineStr"/>
+      <c r="U105" t="inlineStr"/>
+      <c r="V105" t="inlineStr"/>
+      <c r="W105" t="inlineStr"/>
+      <c r="X105" t="inlineStr"/>
+      <c r="Y105" t="inlineStr"/>
+      <c r="Z105" t="inlineStr"/>
+      <c r="AA105" t="inlineStr"/>
+      <c r="AB105" t="inlineStr"/>
+      <c r="AC105" t="inlineStr"/>
+      <c r="AD105" t="inlineStr"/>
+      <c r="AE105" t="inlineStr"/>
+      <c r="AF105" t="inlineStr"/>
+      <c r="AG105" t="inlineStr"/>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr"/>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>sample-1</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr"/>
+      <c r="D106" t="inlineStr"/>
+      <c r="E106" t="inlineStr"/>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>1767177966_JAGADEESH-M-FlowCV-Resume-20251212.pdf</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr"/>
+      <c r="H106" t="inlineStr"/>
+      <c r="I106" t="inlineStr"/>
+      <c r="J106" t="inlineStr"/>
+      <c r="K106" t="inlineStr"/>
+      <c r="L106" t="inlineStr"/>
+      <c r="M106" t="inlineStr"/>
+      <c r="N106" t="inlineStr"/>
+      <c r="O106" t="inlineStr"/>
+      <c r="P106" t="inlineStr"/>
+      <c r="Q106" t="inlineStr"/>
+      <c r="R106" t="inlineStr"/>
+      <c r="S106" t="inlineStr"/>
+      <c r="T106" t="inlineStr"/>
+      <c r="U106" t="inlineStr"/>
+      <c r="V106" t="inlineStr"/>
+      <c r="W106" t="inlineStr"/>
+      <c r="X106" t="inlineStr"/>
+      <c r="Y106" t="inlineStr"/>
+      <c r="Z106" t="inlineStr"/>
+      <c r="AA106" t="inlineStr"/>
+      <c r="AB106" t="inlineStr"/>
+      <c r="AC106" t="inlineStr"/>
+      <c r="AD106" t="inlineStr"/>
+      <c r="AE106" t="inlineStr"/>
+      <c r="AF106" t="inlineStr"/>
+      <c r="AG106" t="inlineStr"/>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr"/>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>sample 2</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr"/>
+      <c r="D107" t="inlineStr"/>
+      <c r="E107" t="inlineStr"/>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>1767177991_JAGADEESH-M-FlowCV-Resume-20251212.pdf</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr"/>
+      <c r="H107" t="inlineStr"/>
+      <c r="I107" t="inlineStr"/>
+      <c r="J107" t="inlineStr"/>
+      <c r="K107" t="inlineStr"/>
+      <c r="L107" t="inlineStr"/>
+      <c r="M107" t="inlineStr"/>
+      <c r="N107" t="inlineStr"/>
+      <c r="O107" t="inlineStr"/>
+      <c r="P107" t="inlineStr"/>
+      <c r="Q107" t="inlineStr"/>
+      <c r="R107" t="inlineStr"/>
+      <c r="S107" t="inlineStr"/>
+      <c r="T107" t="inlineStr"/>
+      <c r="U107" t="inlineStr"/>
+      <c r="V107" t="inlineStr"/>
+      <c r="W107" t="inlineStr"/>
+      <c r="X107" t="inlineStr"/>
+      <c r="Y107" t="inlineStr"/>
+      <c r="Z107" t="inlineStr"/>
+      <c r="AA107" t="inlineStr"/>
+      <c r="AB107" t="inlineStr"/>
+      <c r="AC107" t="inlineStr"/>
+      <c r="AD107" t="inlineStr"/>
+      <c r="AE107" t="inlineStr"/>
+      <c r="AF107" t="inlineStr"/>
+      <c r="AG107" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Integrate Guhatek API as primary data source and add monthly filter to User Activity
- Replace Excel with Guhatek API as primary data source for applicants
- Add TokenManager class for JWT token caching (10 min expiry)
- Filter out null/incomplete applicant records from API
- Add monthly dropdown filter to User Activity section
- Fix date parsing for MM/DD/YYYY Excel format
- Add fallback to Excel if API fails
- Remove manual Fetch from API button (now auto-loads)
</commit_message>
<xml_diff>
--- a/my_app/uploads/data.xlsx
+++ b/my_app/uploads/data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG107"/>
+  <dimension ref="A1:AG109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:AF104"/>
@@ -1278,7 +1278,11 @@
       <c r="X7" t="inlineStr"/>
       <c r="Y7" t="inlineStr"/>
       <c r="Z7" t="inlineStr"/>
-      <c r="AA7" t="inlineStr"/>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>{"Communication":"good","Technical Assessment":"good","Problem-Solving":"good","Overall Potential":"good","Recommendation":"Proceed Round 2"}</t>
+        </is>
+      </c>
       <c r="AB7" t="inlineStr"/>
       <c r="AC7" t="inlineStr"/>
       <c r="AD7" t="inlineStr"/>
@@ -1288,7 +1292,11 @@
           <t>No</t>
         </is>
       </c>
-      <c r="AG7" t="inlineStr"/>
+      <c r="AG7" t="inlineStr">
+        <is>
+          <t>ashwin</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -10266,6 +10274,164 @@
       <c r="AF107" t="inlineStr"/>
       <c r="AG107" t="inlineStr"/>
     </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>2025-12-23 00:00:00</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Jeenusha John</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>jkhjjjqq@example.com</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>9999999992</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>https://linkedin.com/in/jeenusha</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>4a4de728-6ddd-4f48-9441-b3ac101b2291-JeenushaJohn_Resume.pdf</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>SRE</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>Engineer</t>
+        </is>
+      </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>ABC Corp</t>
+        </is>
+      </c>
+      <c r="J108" t="inlineStr">
+        <is>
+          <t>5 years</t>
+        </is>
+      </c>
+      <c r="K108" t="inlineStr">
+        <is>
+          <t>Chennai</t>
+        </is>
+      </c>
+      <c r="L108" t="inlineStr">
+        <is>
+          <t>Any</t>
+        </is>
+      </c>
+      <c r="M108" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="N108" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="O108" t="inlineStr">
+        <is>
+          <t>30 days</t>
+        </is>
+      </c>
+      <c r="P108" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="Q108" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="R108" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S108" t="inlineStr"/>
+      <c r="T108" t="inlineStr"/>
+      <c r="U108" t="inlineStr"/>
+      <c r="V108" t="inlineStr">
+        <is>
+          <t>Applied</t>
+        </is>
+      </c>
+      <c r="W108" t="inlineStr">
+        <is>
+          <t>Proceed Further</t>
+        </is>
+      </c>
+      <c r="X108" t="inlineStr"/>
+      <c r="Y108" t="inlineStr"/>
+      <c r="Z108" t="inlineStr"/>
+      <c r="AA108" t="inlineStr"/>
+      <c r="AB108" t="inlineStr"/>
+      <c r="AC108" t="inlineStr"/>
+      <c r="AD108" t="inlineStr"/>
+      <c r="AE108" t="inlineStr"/>
+      <c r="AF108" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AG108" t="inlineStr"/>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr"/>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>JAGADEESH M</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr"/>
+      <c r="D109" t="inlineStr"/>
+      <c r="E109" t="inlineStr"/>
+      <c r="F109" t="inlineStr"/>
+      <c r="G109" t="inlineStr"/>
+      <c r="H109" t="inlineStr"/>
+      <c r="I109" t="inlineStr"/>
+      <c r="J109" t="inlineStr"/>
+      <c r="K109" t="inlineStr"/>
+      <c r="L109" t="inlineStr"/>
+      <c r="M109" t="inlineStr"/>
+      <c r="N109" t="inlineStr"/>
+      <c r="O109" t="inlineStr"/>
+      <c r="P109" t="inlineStr"/>
+      <c r="Q109" t="inlineStr"/>
+      <c r="R109" t="inlineStr"/>
+      <c r="S109" t="inlineStr"/>
+      <c r="T109" t="inlineStr"/>
+      <c r="U109" t="inlineStr"/>
+      <c r="V109" t="inlineStr"/>
+      <c r="W109" t="inlineStr"/>
+      <c r="X109" t="inlineStr"/>
+      <c r="Y109" t="inlineStr"/>
+      <c r="Z109" t="inlineStr"/>
+      <c r="AA109" t="inlineStr"/>
+      <c r="AB109" t="inlineStr"/>
+      <c r="AC109" t="inlineStr"/>
+      <c r="AD109" t="inlineStr"/>
+      <c r="AE109" t="inlineStr"/>
+      <c r="AF109" t="inlineStr"/>
+      <c r="AG109" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: Integrate Guhatek PATCH API for candidate updates
- Add field mapping (PORTAL_TO_API_FIELD_MAP) for portal to API conversion
- Add update_applicant_via_api() to call PATCH endpoint
- Enhanced GET /api/data to include _api_id and screening data from API
- Enhanced PUT /api/data to sync updates to Guhatek API
- Add updateCandidateData() helper in frontend for API sync
- Hide _api_id column from table display
- Format dates and parse JSON remarks in Edit modal for readability
- Update documentation with PATCH integration details
</commit_message>
<xml_diff>
--- a/my_app/uploads/data.xlsx
+++ b/my_app/uploads/data.xlsx
@@ -591,82 +591,82 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-18 18:48:54</t>
+          <t>2025-12-23T00:00:00.000Z</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>John Doe</t>
+          <t>Jeenusha John</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>john.doe@example.com</t>
+          <t>jkhjjjqq@example.com</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>9876543210</t>
+          <t>9999999992</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/johndoe</t>
+          <t>https://linkedin.com/in/jeenusha</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Resume_JohnDoe_2.pdf</t>
+          <t>4a4de728-6ddd-4f48-9441-b3ac101b2291-JeenushaJohn_Resume.pdf</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Software Developer</t>
+          <t>SRE</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Junior Developer</t>
+          <t>Engineer</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Tech Solutions Inc.</t>
+          <t>ABC Corp</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2-3 years</t>
+          <t>5</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Chennai</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Any</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>800000</t>
+          <t>10</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>1200000</t>
+          <t>15</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>30 days</t>
+          <t>30</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
@@ -680,48 +680,20 @@
         </is>
       </c>
       <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>AWS Certified Developer</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>Employee Referral</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>Scheduled</t>
-        </is>
-      </c>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
       <c r="W2" t="inlineStr">
         <is>
           <t>Accepted</t>
         </is>
       </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>Promising candidate</t>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>Candidate performed well in initial screening.</t>
-        </is>
-      </c>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
       <c r="Z2" t="inlineStr"/>
-      <c r="AA2" t="inlineStr">
-        <is>
-          <t>{"Communication":"","Technical Assessment":"","Problem-Solving":"","Overall Potential":"","Recommendation":"Proceed Round 2"}</t>
-        </is>
-      </c>
+      <c r="AA2" t="inlineStr"/>
       <c r="AB2" t="inlineStr"/>
-      <c r="AC2" t="inlineStr">
-        <is>
-          <t>Good problem-solving approach in Round 2.</t>
-        </is>
-      </c>
+      <c r="AC2" t="inlineStr"/>
       <c r="AD2" t="inlineStr"/>
       <c r="AE2" t="inlineStr"/>
       <c r="AF2" t="inlineStr">
@@ -856,11 +828,15 @@
       <c r="Z3" t="inlineStr"/>
       <c r="AA3" t="inlineStr">
         <is>
-          <t>{"Communication":"good","Technical Assessment":"good","Problem-Solving":"good","Overall Potential":"good","Recommendation":"Proceed Round 2"}</t>
+          <t>{"Communication":"","Technical Assessment":"","Problem-Solving":"","Overall Potential":"","Recommendation":"Proceed Round 2"}</t>
         </is>
       </c>
       <c r="AB3" t="inlineStr"/>
-      <c r="AC3" t="inlineStr"/>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>{"Communication":"","Technical Assessment":"","Problem-Solving":"","Overall Potential":"","Recommendation":" very good ","CTC":""}</t>
+        </is>
+      </c>
       <c r="AD3" t="inlineStr">
         <is>
           <t>junior engineering</t>
@@ -874,57 +850,61 @@
       </c>
       <c r="AG3" t="inlineStr">
         <is>
-          <t>ashwin</t>
+          <t>admin</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>12/18/2025</t>
+          <t>2025-12-23T00:00:00.000Z</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Ram</t>
+          <t>Jeenusha John</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>sam.wilson@example.com</t>
+          <t>jkhjjj@example.com</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>7654321098</t>
+          <t>9999999999</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/samwilson</t>
+          <t>https://linkedin.com/in/jeenusha</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Resume_Ram_4.pdf</t>
+          <t>7ae92d4c-aecf-4caf-86cb-61d57e5bdcf3-JeenushaJohn_Resume.pdf</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>UI/UX Designer</t>
+          <t>SRE</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Graphic Designer</t>
+          <t>Engineer</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Creative Designs</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr"/>
+          <t>ABC Corp</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
       <c r="K4" t="inlineStr">
         <is>
           <t>Chennai</t>
@@ -932,24 +912,32 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Chennai</t>
+          <t>Any</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>700000</t>
+          <t>10</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>1000000</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
@@ -958,61 +946,25 @@
         </is>
       </c>
       <c r="S4" t="inlineStr"/>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>Adobe Certified Expert</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>Campus Recruitment</t>
-        </is>
-      </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>Applied</t>
-        </is>
-      </c>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
       <c r="W4" t="inlineStr">
         <is>
-          <t>Rejected</t>
-        </is>
-      </c>
-      <c r="X4" t="inlineStr">
-        <is>
-          <t>Not enough experience</t>
-        </is>
-      </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="Z4" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+          <t>Accepted</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
       <c r="AA4" t="inlineStr"/>
-      <c r="AB4" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="AB4" t="inlineStr"/>
       <c r="AC4" t="inlineStr"/>
-      <c r="AD4" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="AE4" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="AD4" t="inlineStr"/>
+      <c r="AE4" t="inlineStr"/>
       <c r="AF4" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="AG4" t="inlineStr"/>

</xml_diff>

<commit_message>
feat: Integrate Guhatek POST API for adding new candidates
- Add create_applicant_via_api() helper for POST /api/applications
- Enhanced add_data() to sync new candidates to Guhatek API
- Uploads resume files to Guhatek MinIO storage
- Store returned _api_id for future PATCH updates
- Falls back to local Excel if API fails
- Frontend shows API sync status in success notification
- Updated documentation with POST integration details
</commit_message>
<xml_diff>
--- a/my_app/uploads/data.xlsx
+++ b/my_app/uploads/data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG109"/>
+  <dimension ref="A1:AG112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:AF104"/>
@@ -682,12 +682,12 @@
       <c r="S2" t="inlineStr"/>
       <c r="T2" t="inlineStr"/>
       <c r="U2" t="inlineStr"/>
-      <c r="V2" t="inlineStr"/>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>Accepted</t>
-        </is>
-      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>Offer</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr"/>
       <c r="X2" t="inlineStr"/>
       <c r="Y2" t="inlineStr"/>
       <c r="Z2" t="inlineStr"/>
@@ -10384,6 +10384,127 @@
       <c r="AF109" t="inlineStr"/>
       <c r="AG109" t="inlineStr"/>
     </row>
+    <row r="110">
+      <c r="A110" t="inlineStr"/>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>JAGADEESH M</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr"/>
+      <c r="D110" t="inlineStr"/>
+      <c r="E110" t="inlineStr"/>
+      <c r="F110" t="inlineStr"/>
+      <c r="G110" t="inlineStr"/>
+      <c r="H110" t="inlineStr"/>
+      <c r="I110" t="inlineStr"/>
+      <c r="J110" t="inlineStr"/>
+      <c r="K110" t="inlineStr"/>
+      <c r="L110" t="inlineStr"/>
+      <c r="M110" t="inlineStr"/>
+      <c r="N110" t="inlineStr"/>
+      <c r="O110" t="inlineStr"/>
+      <c r="P110" t="inlineStr"/>
+      <c r="Q110" t="inlineStr"/>
+      <c r="R110" t="inlineStr"/>
+      <c r="S110" t="inlineStr"/>
+      <c r="T110" t="inlineStr"/>
+      <c r="U110" t="inlineStr"/>
+      <c r="V110" t="inlineStr"/>
+      <c r="W110" t="inlineStr"/>
+      <c r="X110" t="inlineStr"/>
+      <c r="Y110" t="inlineStr"/>
+      <c r="Z110" t="inlineStr"/>
+      <c r="AA110" t="inlineStr"/>
+      <c r="AB110" t="inlineStr"/>
+      <c r="AC110" t="inlineStr"/>
+      <c r="AD110" t="inlineStr"/>
+      <c r="AE110" t="inlineStr"/>
+      <c r="AF110" t="inlineStr"/>
+      <c r="AG110" t="inlineStr"/>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr"/>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>JAGADEESH M</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr"/>
+      <c r="D111" t="inlineStr"/>
+      <c r="E111" t="inlineStr"/>
+      <c r="F111" t="inlineStr"/>
+      <c r="G111" t="inlineStr"/>
+      <c r="H111" t="inlineStr"/>
+      <c r="I111" t="inlineStr"/>
+      <c r="J111" t="inlineStr"/>
+      <c r="K111" t="inlineStr"/>
+      <c r="L111" t="inlineStr"/>
+      <c r="M111" t="inlineStr"/>
+      <c r="N111" t="inlineStr"/>
+      <c r="O111" t="inlineStr"/>
+      <c r="P111" t="inlineStr"/>
+      <c r="Q111" t="inlineStr"/>
+      <c r="R111" t="inlineStr"/>
+      <c r="S111" t="inlineStr"/>
+      <c r="T111" t="inlineStr"/>
+      <c r="U111" t="inlineStr"/>
+      <c r="V111" t="inlineStr"/>
+      <c r="W111" t="inlineStr"/>
+      <c r="X111" t="inlineStr"/>
+      <c r="Y111" t="inlineStr"/>
+      <c r="Z111" t="inlineStr"/>
+      <c r="AA111" t="inlineStr"/>
+      <c r="AB111" t="inlineStr"/>
+      <c r="AC111" t="inlineStr"/>
+      <c r="AD111" t="inlineStr"/>
+      <c r="AE111" t="inlineStr"/>
+      <c r="AF111" t="inlineStr"/>
+      <c r="AG111" t="inlineStr"/>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr"/>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>JAGADEESH M</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr"/>
+      <c r="D112" t="inlineStr"/>
+      <c r="E112" t="inlineStr"/>
+      <c r="F112" t="inlineStr"/>
+      <c r="G112" t="inlineStr"/>
+      <c r="H112" t="inlineStr"/>
+      <c r="I112" t="inlineStr"/>
+      <c r="J112" t="inlineStr"/>
+      <c r="K112" t="inlineStr"/>
+      <c r="L112" t="inlineStr"/>
+      <c r="M112" t="inlineStr"/>
+      <c r="N112" t="inlineStr"/>
+      <c r="O112" t="inlineStr"/>
+      <c r="P112" t="inlineStr"/>
+      <c r="Q112" t="inlineStr"/>
+      <c r="R112" t="inlineStr"/>
+      <c r="S112" t="inlineStr"/>
+      <c r="T112" t="inlineStr">
+        <is>
+          <t>nill</t>
+        </is>
+      </c>
+      <c r="U112" t="inlineStr"/>
+      <c r="V112" t="inlineStr"/>
+      <c r="W112" t="inlineStr"/>
+      <c r="X112" t="inlineStr"/>
+      <c r="Y112" t="inlineStr"/>
+      <c r="Z112" t="inlineStr"/>
+      <c r="AA112" t="inlineStr"/>
+      <c r="AB112" t="inlineStr"/>
+      <c r="AC112" t="inlineStr"/>
+      <c r="AD112" t="inlineStr"/>
+      <c r="AE112" t="inlineStr"/>
+      <c r="AF112" t="inlineStr"/>
+      <c r="AG112" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: Fix POST API integration for adding new candidates
- Fixed field name lookup to handle both with-space and without-space versions
  (e.g., EmailID vs Email ID) since frontend uses IDs without spaces
- Only include non-empty fields in API payload to avoid 500 errors
- Handle resume requirement: API requires resume file, skip sync if missing
- Improved logging and error messages for better debugging
- Graceful fallback to local Excel storage when API sync fails
</commit_message>
<xml_diff>
--- a/my_app/uploads/data.xlsx
+++ b/my_app/uploads/data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG112"/>
+  <dimension ref="A1:AG132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:AF104"/>
@@ -10505,6 +10505,894 @@
       <c r="AF112" t="inlineStr"/>
       <c r="AG112" t="inlineStr"/>
     </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>2026-01-09 16:51:24</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>JAGADEESH M</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr"/>
+      <c r="D113" t="inlineStr"/>
+      <c r="E113" t="inlineStr"/>
+      <c r="F113" t="inlineStr"/>
+      <c r="G113" t="inlineStr"/>
+      <c r="H113" t="inlineStr"/>
+      <c r="I113" t="inlineStr"/>
+      <c r="J113" t="inlineStr"/>
+      <c r="K113" t="inlineStr"/>
+      <c r="L113" t="inlineStr"/>
+      <c r="M113" t="inlineStr"/>
+      <c r="N113" t="inlineStr"/>
+      <c r="O113" t="inlineStr"/>
+      <c r="P113" t="inlineStr"/>
+      <c r="Q113" t="inlineStr"/>
+      <c r="R113" t="inlineStr"/>
+      <c r="S113" t="inlineStr"/>
+      <c r="T113" t="inlineStr"/>
+      <c r="U113" t="inlineStr"/>
+      <c r="V113" t="inlineStr"/>
+      <c r="W113" t="inlineStr"/>
+      <c r="X113" t="inlineStr"/>
+      <c r="Y113" t="inlineStr"/>
+      <c r="Z113" t="inlineStr"/>
+      <c r="AA113" t="inlineStr"/>
+      <c r="AB113" t="inlineStr"/>
+      <c r="AC113" t="inlineStr"/>
+      <c r="AD113" t="inlineStr"/>
+      <c r="AE113" t="inlineStr"/>
+      <c r="AF113" t="inlineStr"/>
+      <c r="AG113" t="inlineStr"/>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>2026-01-09 16:57:10</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Test Candidate API</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr"/>
+      <c r="D114" t="inlineStr"/>
+      <c r="E114" t="inlineStr"/>
+      <c r="F114" t="inlineStr"/>
+      <c r="G114" t="inlineStr"/>
+      <c r="H114" t="inlineStr"/>
+      <c r="I114" t="inlineStr"/>
+      <c r="J114" t="inlineStr"/>
+      <c r="K114" t="inlineStr"/>
+      <c r="L114" t="inlineStr"/>
+      <c r="M114" t="inlineStr"/>
+      <c r="N114" t="inlineStr"/>
+      <c r="O114" t="inlineStr"/>
+      <c r="P114" t="inlineStr"/>
+      <c r="Q114" t="inlineStr"/>
+      <c r="R114" t="inlineStr"/>
+      <c r="S114" t="inlineStr"/>
+      <c r="T114" t="inlineStr"/>
+      <c r="U114" t="inlineStr"/>
+      <c r="V114" t="inlineStr"/>
+      <c r="W114" t="inlineStr"/>
+      <c r="X114" t="inlineStr"/>
+      <c r="Y114" t="inlineStr"/>
+      <c r="Z114" t="inlineStr"/>
+      <c r="AA114" t="inlineStr"/>
+      <c r="AB114" t="inlineStr"/>
+      <c r="AC114" t="inlineStr"/>
+      <c r="AD114" t="inlineStr"/>
+      <c r="AE114" t="inlineStr"/>
+      <c r="AF114" t="inlineStr"/>
+      <c r="AG114" t="inlineStr"/>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>2026-01-09 17:02:02</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Test Candidate</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr"/>
+      <c r="D115" t="inlineStr"/>
+      <c r="E115" t="inlineStr"/>
+      <c r="F115" t="inlineStr"/>
+      <c r="G115" t="inlineStr"/>
+      <c r="H115" t="inlineStr"/>
+      <c r="I115" t="inlineStr"/>
+      <c r="J115" t="inlineStr"/>
+      <c r="K115" t="inlineStr"/>
+      <c r="L115" t="inlineStr"/>
+      <c r="M115" t="inlineStr"/>
+      <c r="N115" t="inlineStr"/>
+      <c r="O115" t="inlineStr"/>
+      <c r="P115" t="inlineStr"/>
+      <c r="Q115" t="inlineStr"/>
+      <c r="R115" t="inlineStr"/>
+      <c r="S115" t="inlineStr"/>
+      <c r="T115" t="inlineStr"/>
+      <c r="U115" t="inlineStr"/>
+      <c r="V115" t="inlineStr"/>
+      <c r="W115" t="inlineStr"/>
+      <c r="X115" t="inlineStr"/>
+      <c r="Y115" t="inlineStr"/>
+      <c r="Z115" t="inlineStr"/>
+      <c r="AA115" t="inlineStr"/>
+      <c r="AB115" t="inlineStr"/>
+      <c r="AC115" t="inlineStr"/>
+      <c r="AD115" t="inlineStr"/>
+      <c r="AE115" t="inlineStr"/>
+      <c r="AF115" t="inlineStr"/>
+      <c r="AG115" t="inlineStr"/>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>2026-01-09 17:02:23</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Test Candidate with File</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr"/>
+      <c r="D116" t="inlineStr"/>
+      <c r="E116" t="inlineStr"/>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>1767958343_dummy_resume.pdf</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr"/>
+      <c r="H116" t="inlineStr"/>
+      <c r="I116" t="inlineStr"/>
+      <c r="J116" t="inlineStr"/>
+      <c r="K116" t="inlineStr"/>
+      <c r="L116" t="inlineStr"/>
+      <c r="M116" t="inlineStr"/>
+      <c r="N116" t="inlineStr"/>
+      <c r="O116" t="inlineStr"/>
+      <c r="P116" t="inlineStr"/>
+      <c r="Q116" t="inlineStr"/>
+      <c r="R116" t="inlineStr"/>
+      <c r="S116" t="inlineStr"/>
+      <c r="T116" t="inlineStr"/>
+      <c r="U116" t="inlineStr"/>
+      <c r="V116" t="inlineStr"/>
+      <c r="W116" t="inlineStr"/>
+      <c r="X116" t="inlineStr"/>
+      <c r="Y116" t="inlineStr"/>
+      <c r="Z116" t="inlineStr"/>
+      <c r="AA116" t="inlineStr"/>
+      <c r="AB116" t="inlineStr"/>
+      <c r="AC116" t="inlineStr"/>
+      <c r="AD116" t="inlineStr"/>
+      <c r="AE116" t="inlineStr"/>
+      <c r="AF116" t="inlineStr"/>
+      <c r="AG116" t="inlineStr"/>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>2026-01-09 17:03:01</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Test Candidate with File</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr"/>
+      <c r="D117" t="inlineStr"/>
+      <c r="E117" t="inlineStr"/>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>1767958381_dummy_resume.pdf</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr"/>
+      <c r="H117" t="inlineStr"/>
+      <c r="I117" t="inlineStr"/>
+      <c r="J117" t="inlineStr"/>
+      <c r="K117" t="inlineStr"/>
+      <c r="L117" t="inlineStr"/>
+      <c r="M117" t="inlineStr"/>
+      <c r="N117" t="inlineStr"/>
+      <c r="O117" t="inlineStr"/>
+      <c r="P117" t="inlineStr"/>
+      <c r="Q117" t="inlineStr"/>
+      <c r="R117" t="inlineStr"/>
+      <c r="S117" t="inlineStr"/>
+      <c r="T117" t="inlineStr"/>
+      <c r="U117" t="inlineStr"/>
+      <c r="V117" t="inlineStr"/>
+      <c r="W117" t="inlineStr"/>
+      <c r="X117" t="inlineStr"/>
+      <c r="Y117" t="inlineStr"/>
+      <c r="Z117" t="inlineStr"/>
+      <c r="AA117" t="inlineStr"/>
+      <c r="AB117" t="inlineStr"/>
+      <c r="AC117" t="inlineStr"/>
+      <c r="AD117" t="inlineStr"/>
+      <c r="AE117" t="inlineStr"/>
+      <c r="AF117" t="inlineStr"/>
+      <c r="AG117" t="inlineStr"/>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>2026-01-09 17:03:40</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Test Candidate with File</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr"/>
+      <c r="D118" t="inlineStr"/>
+      <c r="E118" t="inlineStr"/>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>1767958420_dummy_resume.pdf</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr"/>
+      <c r="H118" t="inlineStr"/>
+      <c r="I118" t="inlineStr"/>
+      <c r="J118" t="inlineStr"/>
+      <c r="K118" t="inlineStr"/>
+      <c r="L118" t="inlineStr"/>
+      <c r="M118" t="inlineStr"/>
+      <c r="N118" t="inlineStr"/>
+      <c r="O118" t="inlineStr"/>
+      <c r="P118" t="inlineStr"/>
+      <c r="Q118" t="inlineStr"/>
+      <c r="R118" t="inlineStr"/>
+      <c r="S118" t="inlineStr"/>
+      <c r="T118" t="inlineStr"/>
+      <c r="U118" t="inlineStr"/>
+      <c r="V118" t="inlineStr"/>
+      <c r="W118" t="inlineStr"/>
+      <c r="X118" t="inlineStr"/>
+      <c r="Y118" t="inlineStr"/>
+      <c r="Z118" t="inlineStr"/>
+      <c r="AA118" t="inlineStr"/>
+      <c r="AB118" t="inlineStr"/>
+      <c r="AC118" t="inlineStr"/>
+      <c r="AD118" t="inlineStr"/>
+      <c r="AE118" t="inlineStr"/>
+      <c r="AF118" t="inlineStr"/>
+      <c r="AG118" t="inlineStr"/>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>2026-01-09 17:09:32</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr"/>
+      <c r="C119" t="inlineStr"/>
+      <c r="D119" t="inlineStr"/>
+      <c r="E119" t="inlineStr"/>
+      <c r="F119" t="inlineStr"/>
+      <c r="G119" t="inlineStr"/>
+      <c r="H119" t="inlineStr"/>
+      <c r="I119" t="inlineStr"/>
+      <c r="J119" t="inlineStr"/>
+      <c r="K119" t="inlineStr"/>
+      <c r="L119" t="inlineStr"/>
+      <c r="M119" t="inlineStr"/>
+      <c r="N119" t="inlineStr"/>
+      <c r="O119" t="inlineStr"/>
+      <c r="P119" t="inlineStr"/>
+      <c r="Q119" t="inlineStr"/>
+      <c r="R119" t="inlineStr"/>
+      <c r="S119" t="inlineStr"/>
+      <c r="T119" t="inlineStr"/>
+      <c r="U119" t="inlineStr"/>
+      <c r="V119" t="inlineStr"/>
+      <c r="W119" t="inlineStr"/>
+      <c r="X119" t="inlineStr"/>
+      <c r="Y119" t="inlineStr"/>
+      <c r="Z119" t="inlineStr"/>
+      <c r="AA119" t="inlineStr"/>
+      <c r="AB119" t="inlineStr"/>
+      <c r="AC119" t="inlineStr"/>
+      <c r="AD119" t="inlineStr"/>
+      <c r="AE119" t="inlineStr"/>
+      <c r="AF119" t="inlineStr"/>
+      <c r="AG119" t="inlineStr"/>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>2026-01-09 17:10:32</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>API Test User 2</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr"/>
+      <c r="D120" t="inlineStr"/>
+      <c r="E120" t="inlineStr"/>
+      <c r="F120" t="inlineStr"/>
+      <c r="G120" t="inlineStr"/>
+      <c r="H120" t="inlineStr"/>
+      <c r="I120" t="inlineStr"/>
+      <c r="J120" t="inlineStr"/>
+      <c r="K120" t="inlineStr"/>
+      <c r="L120" t="inlineStr"/>
+      <c r="M120" t="inlineStr"/>
+      <c r="N120" t="inlineStr"/>
+      <c r="O120" t="inlineStr"/>
+      <c r="P120" t="inlineStr"/>
+      <c r="Q120" t="inlineStr"/>
+      <c r="R120" t="inlineStr"/>
+      <c r="S120" t="inlineStr"/>
+      <c r="T120" t="inlineStr"/>
+      <c r="U120" t="inlineStr"/>
+      <c r="V120" t="inlineStr"/>
+      <c r="W120" t="inlineStr"/>
+      <c r="X120" t="inlineStr"/>
+      <c r="Y120" t="inlineStr"/>
+      <c r="Z120" t="inlineStr"/>
+      <c r="AA120" t="inlineStr"/>
+      <c r="AB120" t="inlineStr"/>
+      <c r="AC120" t="inlineStr"/>
+      <c r="AD120" t="inlineStr"/>
+      <c r="AE120" t="inlineStr"/>
+      <c r="AF120" t="inlineStr"/>
+      <c r="AG120" t="inlineStr"/>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>2026-01-09 17:11:19</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>API Test User Final</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr"/>
+      <c r="D121" t="inlineStr"/>
+      <c r="E121" t="inlineStr"/>
+      <c r="F121" t="inlineStr"/>
+      <c r="G121" t="inlineStr"/>
+      <c r="H121" t="inlineStr"/>
+      <c r="I121" t="inlineStr"/>
+      <c r="J121" t="inlineStr"/>
+      <c r="K121" t="inlineStr"/>
+      <c r="L121" t="inlineStr"/>
+      <c r="M121" t="inlineStr"/>
+      <c r="N121" t="inlineStr"/>
+      <c r="O121" t="inlineStr"/>
+      <c r="P121" t="inlineStr"/>
+      <c r="Q121" t="inlineStr"/>
+      <c r="R121" t="inlineStr"/>
+      <c r="S121" t="inlineStr"/>
+      <c r="T121" t="inlineStr"/>
+      <c r="U121" t="inlineStr"/>
+      <c r="V121" t="inlineStr"/>
+      <c r="W121" t="inlineStr"/>
+      <c r="X121" t="inlineStr"/>
+      <c r="Y121" t="inlineStr"/>
+      <c r="Z121" t="inlineStr"/>
+      <c r="AA121" t="inlineStr"/>
+      <c r="AB121" t="inlineStr"/>
+      <c r="AC121" t="inlineStr"/>
+      <c r="AD121" t="inlineStr"/>
+      <c r="AE121" t="inlineStr"/>
+      <c r="AF121" t="inlineStr"/>
+      <c r="AG121" t="inlineStr"/>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>2026-01-09 17:12:17</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>API Test User Unique</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr"/>
+      <c r="D122" t="inlineStr"/>
+      <c r="E122" t="inlineStr"/>
+      <c r="F122" t="inlineStr"/>
+      <c r="G122" t="inlineStr"/>
+      <c r="H122" t="inlineStr"/>
+      <c r="I122" t="inlineStr"/>
+      <c r="J122" t="inlineStr"/>
+      <c r="K122" t="inlineStr"/>
+      <c r="L122" t="inlineStr"/>
+      <c r="M122" t="inlineStr"/>
+      <c r="N122" t="inlineStr"/>
+      <c r="O122" t="inlineStr"/>
+      <c r="P122" t="inlineStr"/>
+      <c r="Q122" t="inlineStr"/>
+      <c r="R122" t="inlineStr"/>
+      <c r="S122" t="inlineStr"/>
+      <c r="T122" t="inlineStr"/>
+      <c r="U122" t="inlineStr"/>
+      <c r="V122" t="inlineStr"/>
+      <c r="W122" t="inlineStr"/>
+      <c r="X122" t="inlineStr"/>
+      <c r="Y122" t="inlineStr"/>
+      <c r="Z122" t="inlineStr"/>
+      <c r="AA122" t="inlineStr"/>
+      <c r="AB122" t="inlineStr"/>
+      <c r="AC122" t="inlineStr"/>
+      <c r="AD122" t="inlineStr"/>
+      <c r="AE122" t="inlineStr"/>
+      <c r="AF122" t="inlineStr"/>
+      <c r="AG122" t="inlineStr"/>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>2026-01-09 17:14:04</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>API Test User Final</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr"/>
+      <c r="D123" t="inlineStr"/>
+      <c r="E123" t="inlineStr"/>
+      <c r="F123" t="inlineStr"/>
+      <c r="G123" t="inlineStr"/>
+      <c r="H123" t="inlineStr"/>
+      <c r="I123" t="inlineStr"/>
+      <c r="J123" t="inlineStr"/>
+      <c r="K123" t="inlineStr"/>
+      <c r="L123" t="inlineStr"/>
+      <c r="M123" t="inlineStr"/>
+      <c r="N123" t="inlineStr"/>
+      <c r="O123" t="inlineStr"/>
+      <c r="P123" t="inlineStr"/>
+      <c r="Q123" t="inlineStr"/>
+      <c r="R123" t="inlineStr"/>
+      <c r="S123" t="inlineStr"/>
+      <c r="T123" t="inlineStr"/>
+      <c r="U123" t="inlineStr"/>
+      <c r="V123" t="inlineStr"/>
+      <c r="W123" t="inlineStr"/>
+      <c r="X123" t="inlineStr"/>
+      <c r="Y123" t="inlineStr"/>
+      <c r="Z123" t="inlineStr"/>
+      <c r="AA123" t="inlineStr"/>
+      <c r="AB123" t="inlineStr"/>
+      <c r="AC123" t="inlineStr"/>
+      <c r="AD123" t="inlineStr"/>
+      <c r="AE123" t="inlineStr"/>
+      <c r="AF123" t="inlineStr"/>
+      <c r="AG123" t="inlineStr"/>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>2026-01-09 17:14:34</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>API Test Manual</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>manual_1767959073784@example.com</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>2222222222</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr"/>
+      <c r="F124" t="inlineStr"/>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>DevOps Engineer</t>
+        </is>
+      </c>
+      <c r="H124" t="inlineStr"/>
+      <c r="I124" t="inlineStr"/>
+      <c r="J124" t="inlineStr"/>
+      <c r="K124" t="inlineStr"/>
+      <c r="L124" t="inlineStr"/>
+      <c r="M124" t="inlineStr"/>
+      <c r="N124" t="inlineStr"/>
+      <c r="O124" t="inlineStr"/>
+      <c r="P124" t="inlineStr"/>
+      <c r="Q124" t="inlineStr"/>
+      <c r="R124" t="inlineStr"/>
+      <c r="S124" t="inlineStr"/>
+      <c r="T124" t="inlineStr"/>
+      <c r="U124" t="inlineStr"/>
+      <c r="V124" t="inlineStr"/>
+      <c r="W124" t="inlineStr"/>
+      <c r="X124" t="inlineStr"/>
+      <c r="Y124" t="inlineStr"/>
+      <c r="Z124" t="inlineStr"/>
+      <c r="AA124" t="inlineStr"/>
+      <c r="AB124" t="inlineStr"/>
+      <c r="AC124" t="inlineStr"/>
+      <c r="AD124" t="inlineStr"/>
+      <c r="AE124" t="inlineStr"/>
+      <c r="AF124" t="inlineStr"/>
+      <c r="AG124" t="inlineStr"/>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>2026-01-09 17:18:50</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Fixed API Test</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr"/>
+      <c r="D125" t="inlineStr"/>
+      <c r="E125" t="inlineStr"/>
+      <c r="F125" t="inlineStr"/>
+      <c r="G125" t="inlineStr"/>
+      <c r="H125" t="inlineStr"/>
+      <c r="I125" t="inlineStr"/>
+      <c r="J125" t="inlineStr"/>
+      <c r="K125" t="inlineStr"/>
+      <c r="L125" t="inlineStr"/>
+      <c r="M125" t="inlineStr"/>
+      <c r="N125" t="inlineStr"/>
+      <c r="O125" t="inlineStr"/>
+      <c r="P125" t="inlineStr"/>
+      <c r="Q125" t="inlineStr"/>
+      <c r="R125" t="inlineStr"/>
+      <c r="S125" t="inlineStr"/>
+      <c r="T125" t="inlineStr"/>
+      <c r="U125" t="inlineStr"/>
+      <c r="V125" t="inlineStr"/>
+      <c r="W125" t="inlineStr"/>
+      <c r="X125" t="inlineStr"/>
+      <c r="Y125" t="inlineStr"/>
+      <c r="Z125" t="inlineStr"/>
+      <c r="AA125" t="inlineStr"/>
+      <c r="AB125" t="inlineStr"/>
+      <c r="AC125" t="inlineStr"/>
+      <c r="AD125" t="inlineStr"/>
+      <c r="AE125" t="inlineStr"/>
+      <c r="AF125" t="inlineStr"/>
+      <c r="AG125" t="inlineStr"/>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>2026-01-09 17:19:55</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Fixed API Test</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr"/>
+      <c r="D126" t="inlineStr"/>
+      <c r="E126" t="inlineStr"/>
+      <c r="F126" t="inlineStr"/>
+      <c r="G126" t="inlineStr"/>
+      <c r="H126" t="inlineStr"/>
+      <c r="I126" t="inlineStr"/>
+      <c r="J126" t="inlineStr"/>
+      <c r="K126" t="inlineStr"/>
+      <c r="L126" t="inlineStr"/>
+      <c r="M126" t="inlineStr"/>
+      <c r="N126" t="inlineStr"/>
+      <c r="O126" t="inlineStr"/>
+      <c r="P126" t="inlineStr"/>
+      <c r="Q126" t="inlineStr"/>
+      <c r="R126" t="inlineStr"/>
+      <c r="S126" t="inlineStr"/>
+      <c r="T126" t="inlineStr"/>
+      <c r="U126" t="inlineStr"/>
+      <c r="V126" t="inlineStr"/>
+      <c r="W126" t="inlineStr"/>
+      <c r="X126" t="inlineStr"/>
+      <c r="Y126" t="inlineStr"/>
+      <c r="Z126" t="inlineStr"/>
+      <c r="AA126" t="inlineStr"/>
+      <c r="AB126" t="inlineStr"/>
+      <c r="AC126" t="inlineStr"/>
+      <c r="AD126" t="inlineStr"/>
+      <c r="AE126" t="inlineStr"/>
+      <c r="AF126" t="inlineStr"/>
+      <c r="AG126" t="inlineStr"/>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>2026-01-09 17:23:15</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Final Test</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr"/>
+      <c r="D127" t="inlineStr"/>
+      <c r="E127" t="inlineStr"/>
+      <c r="F127" t="inlineStr"/>
+      <c r="G127" t="inlineStr"/>
+      <c r="H127" t="inlineStr"/>
+      <c r="I127" t="inlineStr"/>
+      <c r="J127" t="inlineStr"/>
+      <c r="K127" t="inlineStr"/>
+      <c r="L127" t="inlineStr"/>
+      <c r="M127" t="inlineStr"/>
+      <c r="N127" t="inlineStr"/>
+      <c r="O127" t="inlineStr"/>
+      <c r="P127" t="inlineStr"/>
+      <c r="Q127" t="inlineStr"/>
+      <c r="R127" t="inlineStr"/>
+      <c r="S127" t="inlineStr"/>
+      <c r="T127" t="inlineStr"/>
+      <c r="U127" t="inlineStr"/>
+      <c r="V127" t="inlineStr"/>
+      <c r="W127" t="inlineStr"/>
+      <c r="X127" t="inlineStr"/>
+      <c r="Y127" t="inlineStr"/>
+      <c r="Z127" t="inlineStr"/>
+      <c r="AA127" t="inlineStr"/>
+      <c r="AB127" t="inlineStr"/>
+      <c r="AC127" t="inlineStr"/>
+      <c r="AD127" t="inlineStr"/>
+      <c r="AE127" t="inlineStr"/>
+      <c r="AF127" t="inlineStr"/>
+      <c r="AG127" t="inlineStr"/>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>2026-01-09 17:25:26</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Observed Test</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr"/>
+      <c r="D128" t="inlineStr"/>
+      <c r="E128" t="inlineStr"/>
+      <c r="F128" t="inlineStr"/>
+      <c r="G128" t="inlineStr"/>
+      <c r="H128" t="inlineStr"/>
+      <c r="I128" t="inlineStr"/>
+      <c r="J128" t="inlineStr"/>
+      <c r="K128" t="inlineStr"/>
+      <c r="L128" t="inlineStr"/>
+      <c r="M128" t="inlineStr"/>
+      <c r="N128" t="inlineStr"/>
+      <c r="O128" t="inlineStr"/>
+      <c r="P128" t="inlineStr"/>
+      <c r="Q128" t="inlineStr"/>
+      <c r="R128" t="inlineStr"/>
+      <c r="S128" t="inlineStr"/>
+      <c r="T128" t="inlineStr"/>
+      <c r="U128" t="inlineStr"/>
+      <c r="V128" t="inlineStr"/>
+      <c r="W128" t="inlineStr"/>
+      <c r="X128" t="inlineStr"/>
+      <c r="Y128" t="inlineStr"/>
+      <c r="Z128" t="inlineStr"/>
+      <c r="AA128" t="inlineStr"/>
+      <c r="AB128" t="inlineStr"/>
+      <c r="AC128" t="inlineStr"/>
+      <c r="AD128" t="inlineStr"/>
+      <c r="AE128" t="inlineStr"/>
+      <c r="AF128" t="inlineStr"/>
+      <c r="AG128" t="inlineStr"/>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>2026-01-09 17:27:36</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>UniqueName12345</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr"/>
+      <c r="D129" t="inlineStr"/>
+      <c r="E129" t="inlineStr"/>
+      <c r="F129" t="inlineStr"/>
+      <c r="G129" t="inlineStr"/>
+      <c r="H129" t="inlineStr"/>
+      <c r="I129" t="inlineStr"/>
+      <c r="J129" t="inlineStr"/>
+      <c r="K129" t="inlineStr"/>
+      <c r="L129" t="inlineStr"/>
+      <c r="M129" t="inlineStr"/>
+      <c r="N129" t="inlineStr"/>
+      <c r="O129" t="inlineStr"/>
+      <c r="P129" t="inlineStr"/>
+      <c r="Q129" t="inlineStr"/>
+      <c r="R129" t="inlineStr"/>
+      <c r="S129" t="inlineStr"/>
+      <c r="T129" t="inlineStr"/>
+      <c r="U129" t="inlineStr"/>
+      <c r="V129" t="inlineStr"/>
+      <c r="W129" t="inlineStr"/>
+      <c r="X129" t="inlineStr"/>
+      <c r="Y129" t="inlineStr"/>
+      <c r="Z129" t="inlineStr"/>
+      <c r="AA129" t="inlineStr"/>
+      <c r="AB129" t="inlineStr"/>
+      <c r="AC129" t="inlineStr"/>
+      <c r="AD129" t="inlineStr"/>
+      <c r="AE129" t="inlineStr"/>
+      <c r="AF129" t="inlineStr"/>
+      <c r="AG129" t="inlineStr"/>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>2026-01-09 17:34:16</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Final Test Candidate</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr"/>
+      <c r="D130" t="inlineStr"/>
+      <c r="E130" t="inlineStr"/>
+      <c r="F130" t="inlineStr"/>
+      <c r="G130" t="inlineStr"/>
+      <c r="H130" t="inlineStr"/>
+      <c r="I130" t="inlineStr"/>
+      <c r="J130" t="inlineStr"/>
+      <c r="K130" t="inlineStr"/>
+      <c r="L130" t="inlineStr"/>
+      <c r="M130" t="inlineStr"/>
+      <c r="N130" t="inlineStr"/>
+      <c r="O130" t="inlineStr"/>
+      <c r="P130" t="inlineStr"/>
+      <c r="Q130" t="inlineStr"/>
+      <c r="R130" t="inlineStr"/>
+      <c r="S130" t="inlineStr"/>
+      <c r="T130" t="inlineStr"/>
+      <c r="U130" t="inlineStr"/>
+      <c r="V130" t="inlineStr"/>
+      <c r="W130" t="inlineStr"/>
+      <c r="X130" t="inlineStr"/>
+      <c r="Y130" t="inlineStr"/>
+      <c r="Z130" t="inlineStr"/>
+      <c r="AA130" t="inlineStr"/>
+      <c r="AB130" t="inlineStr"/>
+      <c r="AC130" t="inlineStr"/>
+      <c r="AD130" t="inlineStr"/>
+      <c r="AE130" t="inlineStr"/>
+      <c r="AF130" t="inlineStr"/>
+      <c r="AG130" t="inlineStr"/>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>2026-01-09 17:35:11</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>Second Test Candidate</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr"/>
+      <c r="D131" t="inlineStr"/>
+      <c r="E131" t="inlineStr"/>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>1767960311_dummy_resume.pdf</t>
+        </is>
+      </c>
+      <c r="G131" t="inlineStr"/>
+      <c r="H131" t="inlineStr"/>
+      <c r="I131" t="inlineStr"/>
+      <c r="J131" t="inlineStr"/>
+      <c r="K131" t="inlineStr"/>
+      <c r="L131" t="inlineStr"/>
+      <c r="M131" t="inlineStr"/>
+      <c r="N131" t="inlineStr"/>
+      <c r="O131" t="inlineStr"/>
+      <c r="P131" t="inlineStr"/>
+      <c r="Q131" t="inlineStr"/>
+      <c r="R131" t="inlineStr"/>
+      <c r="S131" t="inlineStr"/>
+      <c r="T131" t="inlineStr"/>
+      <c r="U131" t="inlineStr"/>
+      <c r="V131" t="inlineStr"/>
+      <c r="W131" t="inlineStr"/>
+      <c r="X131" t="inlineStr"/>
+      <c r="Y131" t="inlineStr"/>
+      <c r="Z131" t="inlineStr"/>
+      <c r="AA131" t="inlineStr"/>
+      <c r="AB131" t="inlineStr"/>
+      <c r="AC131" t="inlineStr"/>
+      <c r="AD131" t="inlineStr"/>
+      <c r="AE131" t="inlineStr"/>
+      <c r="AF131" t="inlineStr"/>
+      <c r="AG131" t="inlineStr"/>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>2026-01-09 17:35:41</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>Final Test Candidate</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr"/>
+      <c r="D132" t="inlineStr"/>
+      <c r="E132" t="inlineStr"/>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>1767960341_resume.pdf</t>
+        </is>
+      </c>
+      <c r="G132" t="inlineStr"/>
+      <c r="H132" t="inlineStr"/>
+      <c r="I132" t="inlineStr"/>
+      <c r="J132" t="inlineStr"/>
+      <c r="K132" t="inlineStr"/>
+      <c r="L132" t="inlineStr"/>
+      <c r="M132" t="inlineStr"/>
+      <c r="N132" t="inlineStr"/>
+      <c r="O132" t="inlineStr"/>
+      <c r="P132" t="inlineStr"/>
+      <c r="Q132" t="inlineStr"/>
+      <c r="R132" t="inlineStr"/>
+      <c r="S132" t="inlineStr"/>
+      <c r="T132" t="inlineStr"/>
+      <c r="U132" t="inlineStr"/>
+      <c r="V132" t="inlineStr"/>
+      <c r="W132" t="inlineStr"/>
+      <c r="X132" t="inlineStr"/>
+      <c r="Y132" t="inlineStr"/>
+      <c r="Z132" t="inlineStr"/>
+      <c r="AA132" t="inlineStr"/>
+      <c r="AB132" t="inlineStr"/>
+      <c r="AC132" t="inlineStr"/>
+      <c r="AD132" t="inlineStr"/>
+      <c r="AE132" t="inlineStr"/>
+      <c r="AF132" t="inlineStr"/>
+      <c r="AG132" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>